<commit_message>
Updated config file and Added Documentation
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -149,15 +149,6 @@
     <t>Manager</t>
   </si>
   <si>
-    <t>kchandrutest05@gmail.com</t>
-  </si>
-  <si>
-    <t>kchandru05@hotmail.com</t>
-  </si>
-  <si>
-    <t>ReqID ReqName Priority Severity Type StartDate EndDate Dstatus DStartDate DEndDate</t>
-  </si>
-  <si>
     <t>ReqID ReqName Priority Severity Type StartDate EndDate  TestCaseStatus TestExecutionStatus TStartDate TEndDate</t>
   </si>
   <si>
@@ -174,40 +165,6 @@
   </si>
   <si>
     <t>ProjectTeam</t>
-  </si>
-  <si>
-    <t>kchandru05@gmail.com;chandru.karunanithi@gramenerit.com</t>
-  </si>
-  <si>
-    <t>&lt;html&gt;
-  &lt;head&gt;  
-    &lt;title&gt;&lt;/title&gt;
-  &lt;/head&gt;
-  &lt;body&gt;
-  &lt;p&gt;&lt;span style="&amp;lsquo;font-size: 14px&amp;rsquo;;"&gt;&lt;span style="&amp;lsquo;font-family: tahoma,geneva,sans-serif&amp;rsquo;;"&gt;Dear &lt;strong&gt;Client&lt;/strong&gt;,&lt;br /&gt;&lt;br /&gt;&amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp;Good Day! Please find the today's status report for &lt;strong&gt;ABC Project&lt;/strong&gt;. Kindly Let us know for any issues/clarifications.&amp;nbsp;&lt;br /&gt;&lt;br /&gt;&amp;nbsp; &amp;nbsp; &amp;nbsp; It is kindly expected from you to act on tasks which needed action from your side. The same has been mentioned in Needed Action column. Please have a look and let us know for any update.&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;table style="&amp;lsquo;width: 500px&amp;rsquo;;" border="&amp;lsquo;1&amp;rsquo;" cellspacing="&amp;lsquo;1&amp;rsquo;" cellpadding="&amp;lsquo;1&amp;rsquo;"&gt;
-&lt;tbody&gt;
-&lt;tr&gt;
-&lt;th&gt;ResourceName&lt;/th&gt;
-&lt;th&gt;ResourceEmail&lt;/th&gt;
-&lt;th&gt;TaskStatus&lt;/th&gt;
-&lt;th&gt;TaskAssigned&lt;/th&gt;
-&lt;th&gt;TaskCompleted&lt;/th&gt;
-&lt;th&gt;TaskPending&lt;/th&gt;
-&lt;th&gt;HoursLogged&lt;/th&gt;
-&lt;th&gt;Next Action&lt;/th&gt;
-&lt;th&gt;ResponsiblePerson&lt;/th&gt;
-&lt;th&gt;Clarifications&lt;/th&gt;
-&lt;th&gt;Risk&lt;/th&gt;
-&lt;th&gt;Comment&lt;/th&gt;
-&lt;/tr&gt;
-{0}
-&lt;/tbody&gt;
-&lt;/table&gt;
-&lt;p&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;span style="&amp;lsquo;font-size: 14px&amp;rsquo;;"&gt;&lt;span style="&amp;lsquo;font-family: tahoma,geneva,sans-serif&amp;rsquo;;"&gt;This is auto generated mail. Please contact Project Manager if any issues&lt;br /&gt;&lt;br /&gt;Regards,&lt;br /&gt;Project Team&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
- &lt;/body&gt;
-&lt;/html&gt;</t>
   </si>
   <si>
     <t>AdhocRequirementList</t>
@@ -352,6 +309,50 @@
   <si>
     <t>StatusReportPath</t>
   </si>
+  <si>
+    <t>ReqID ReqName Priority Severity Type StartDate EndDate DStatus DStartDate DEndDate</t>
+  </si>
+  <si>
+    <t>ba@gmail.com</t>
+  </si>
+  <si>
+    <t>manager@gmail.com</t>
+  </si>
+  <si>
+    <t>projectteam@gmail.com;projectteam1@gmail.com;projectteam2@gmail.com;</t>
+  </si>
+  <si>
+    <t>&lt;html&gt;
+  &lt;head&gt;  
+    &lt;title&gt;&lt;/title&gt;
+  &lt;/head&gt;
+  &lt;body&gt;
+  &lt;p&gt;&lt;span style="&amp;lsquo;font-size: 14px&amp;rsquo;;"&gt;&lt;span style="&amp;lsquo;font-family: tahoma,geneva,sans-serif&amp;rsquo;;"&gt;Dear &lt;strong&gt;Client&lt;/strong&gt;,&lt;br /&gt;&lt;br /&gt;&amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp;Good Day! Please find the today's status report for &lt;strong&gt;ABC Project&lt;/strong&gt;. Kindly Let us know for any issues/clarifications.&amp;nbsp;&lt;br /&gt;&lt;br /&gt;&amp;nbsp; &amp;nbsp; &amp;nbsp; It is kindly expected from you to act on tasks which needed action from your side. The same has been mentioned in Needed Action column. Please have a look and let us know for any update.&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;table style="&amp;lsquo;width: 500px&amp;rsquo;;" border="&amp;lsquo;1&amp;rsquo;" cellspacing="&amp;lsquo;1&amp;rsquo;" cellpadding="&amp;lsquo;1&amp;rsquo;"&gt;
+&lt;tbody&gt;
+&lt;tr&gt;
+&lt;th&gt;ResourceName&lt;/th&gt;
+&lt;th&gt;Role&lt;/th&gt;
+&lt;th&gt;ResourceEmail&lt;/th&gt;
+&lt;th&gt;TaskStatus&lt;/th&gt;
+&lt;th&gt;TaskAssigned&lt;/th&gt;
+&lt;th&gt;TaskCompleted&lt;/th&gt;
+&lt;th&gt;TaskPending&lt;/th&gt;
+&lt;th&gt;HoursLogged&lt;/th&gt;
+&lt;th&gt;Next Action&lt;/th&gt;
+&lt;th&gt;ResponsiblePerson&lt;/th&gt;
+&lt;th&gt;Clarifications&lt;/th&gt;
+&lt;th&gt;Risk&lt;/th&gt;
+&lt;th&gt;Comment&lt;/th&gt;
+&lt;/tr&gt;
+{0}
+&lt;/tbody&gt;
+&lt;/table&gt;
+&lt;p&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;span style="&amp;lsquo;font-size: 14px&amp;rsquo;;"&gt;&lt;span style="&amp;lsquo;font-family: tahoma,geneva,sans-serif&amp;rsquo;;"&gt;This is auto generated mail. Please contact Project Manager if any issues&lt;br /&gt;&lt;br /&gt;Regards,&lt;br /&gt;Project Team&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;
+ &lt;/body&gt;
+&lt;/html&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -360,7 +361,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -378,12 +379,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -403,11 +398,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -422,7 +416,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -430,8 +423,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -713,7 +705,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -763,21 +755,21 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -785,21 +777,21 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1803,14 +1795,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="74.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -1855,7 +1847,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -1863,7 +1855,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="45" x14ac:dyDescent="0.25">
@@ -1871,7 +1863,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="45" x14ac:dyDescent="0.25">
@@ -1879,15 +1871,15 @@
         <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -1897,10 +1889,10 @@
     </row>
     <row r="9" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C9" s="6"/>
     </row>
@@ -1930,7 +1922,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4"/>
     </row>
@@ -1939,7 +1931,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C14" s="4"/>
     </row>
@@ -1948,10 +1940,10 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C16" s="4"/>
     </row>
@@ -1962,41 +1954,41 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="9">
+        <v>39</v>
+      </c>
+      <c r="B18" s="8">
         <v>43337</v>
       </c>
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="10">
+        <v>40</v>
+      </c>
+      <c r="B19" s="9">
         <v>43368</v>
       </c>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="10"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="10">
-        <v>43340</v>
+        <v>41</v>
+      </c>
+      <c r="B21" s="9">
+        <v>43339</v>
       </c>
       <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="10">
+        <v>42</v>
+      </c>
+      <c r="B22" s="9">
         <v>43340</v>
       </c>
       <c r="C22" s="4"/>
@@ -2010,7 +2002,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C24" s="4"/>
     </row>
@@ -2018,17 +2010,17 @@
       <c r="A25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>20</v>
+      <c r="B25" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C26" s="4"/>
     </row>
@@ -2038,7 +2030,7 @@
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B29" s="3">
         <v>8</v>
@@ -2047,7 +2039,7 @@
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B31" s="3">
         <v>21</v>
@@ -3020,11 +3012,8 @@
     <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1017" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>